<commit_message>
updated pom and users pages
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/ptsTestData.xlsx
+++ b/src/test/resources/testdata/ptsTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mroads\eclipse-workspace\PTSNew\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A4C6507-1860-4394-850E-785565F71027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADCFFCA5-F579-4183-8614-77CFE41FAEDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0FA2E9B5-5E9F-4473-9BAF-AA72573A5FDA}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7875" xr2:uid="{0FA2E9B5-5E9F-4473-9BAF-AA72573A5FDA}"/>
   </bookViews>
   <sheets>
     <sheet name="userCreate" sheetId="1" r:id="rId1"/>
@@ -99,16 +99,16 @@
     <t>Timesheet Employee</t>
   </si>
   <si>
-    <t>auto eight</t>
-  </si>
-  <si>
-    <t>9000000008</t>
-  </si>
-  <si>
-    <t>gautham.auto8@yopmail.com</t>
-  </si>
-  <si>
-    <t>1-1-108</t>
+    <t>auto nineteen</t>
+  </si>
+  <si>
+    <t>9000000019</t>
+  </si>
+  <si>
+    <t>gautham.auto19@yopmail.com</t>
+  </si>
+  <si>
+    <t>1-1-119</t>
   </si>
 </sst>
 </file>
@@ -474,7 +474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B84F864E-C3CF-4F75-AC05-44E39AE68134}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>

</xml_diff>